<commit_message>
new variable and graphs
</commit_message>
<xml_diff>
--- a/aemet_vino_check3.xlsx
+++ b/aemet_vino_check3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,6 +469,11 @@
           <t>humedad_relativa_manual</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>precipitacion_media_anual_ene_dic</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -490,6 +495,9 @@
       <c r="G2" t="n">
         <v>32.4438915947852</v>
       </c>
+      <c r="H2" t="n">
+        <v>8.699999999999999</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -511,6 +519,9 @@
       <c r="G3" t="n">
         <v>28.05630124065878</v>
       </c>
+      <c r="H3" t="n">
+        <v>42.55384615384616</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -532,6 +543,9 @@
       <c r="G4" t="n">
         <v>37.33766640887496</v>
       </c>
+      <c r="H4" t="n">
+        <v>57.38461538461539</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -553,6 +567,9 @@
       <c r="G5" t="n">
         <v>34.95929932185567</v>
       </c>
+      <c r="H5" t="n">
+        <v>21.175</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -574,6 +591,9 @@
       <c r="G6" t="n">
         <v>39.63943226933223</v>
       </c>
+      <c r="H6" t="n">
+        <v>46.175</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -595,6 +615,9 @@
       <c r="G7" t="n">
         <v>35.60955590342604</v>
       </c>
+      <c r="H7" t="n">
+        <v>26.91111111111111</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -618,6 +641,9 @@
       <c r="G8" t="n">
         <v>36.06557291431047</v>
       </c>
+      <c r="H8" t="n">
+        <v>43.41818181818182</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -641,6 +667,9 @@
       <c r="G9" t="n">
         <v>37.87143878520988</v>
       </c>
+      <c r="H9" t="n">
+        <v>36.50769230769231</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -664,6 +693,9 @@
       <c r="G10" t="n">
         <v>37.59847301562555</v>
       </c>
+      <c r="H10" t="n">
+        <v>45.66153846153846</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -687,6 +719,9 @@
       <c r="G11" t="n">
         <v>34.73312498065534</v>
       </c>
+      <c r="H11" t="n">
+        <v>62.63076923076923</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -710,6 +745,9 @@
       <c r="G12" t="n">
         <v>40.18709050779317</v>
       </c>
+      <c r="H12" t="n">
+        <v>59.8923076923077</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -733,6 +771,9 @@
       <c r="G13" t="n">
         <v>39.46491479156489</v>
       </c>
+      <c r="H13" t="n">
+        <v>38.06153846153846</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -756,6 +797,9 @@
       <c r="G14" t="n">
         <v>36.65902965263522</v>
       </c>
+      <c r="H14" t="n">
+        <v>65.1076923076923</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -779,6 +823,9 @@
       <c r="G15" t="n">
         <v>36.95686151280452</v>
       </c>
+      <c r="H15" t="n">
+        <v>35.56923076923077</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -802,6 +849,9 @@
       <c r="G16" t="n">
         <v>41.01433841604756</v>
       </c>
+      <c r="H16" t="n">
+        <v>81.16923076923078</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -825,6 +875,9 @@
       <c r="G17" t="n">
         <v>36.96039560124134</v>
       </c>
+      <c r="H17" t="n">
+        <v>50.27692307692308</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -848,6 +901,9 @@
       <c r="G18" t="n">
         <v>42.04511643552633</v>
       </c>
+      <c r="H18" t="n">
+        <v>61.23076923076923</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -871,6 +927,9 @@
       <c r="G19" t="n">
         <v>38.71203146508528</v>
       </c>
+      <c r="H19" t="n">
+        <v>50.8923076923077</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -894,6 +953,9 @@
       <c r="G20" t="n">
         <v>38.06939075640929</v>
       </c>
+      <c r="H20" t="n">
+        <v>47.84615384615385</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -917,6 +979,9 @@
       <c r="G21" t="n">
         <v>35.8790911491291</v>
       </c>
+      <c r="H21" t="n">
+        <v>35.22</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -939,6 +1004,9 @@
       </c>
       <c r="G22" t="n">
         <v>38.25732721188101</v>
+      </c>
+      <c r="H22" t="n">
+        <v>34.72727272727273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>